<commit_message>
Update Excel data files and adjust execution counts in master analysis notebook
- Updated `highest_toxicity_records.xlsx`, `operator_shares_by_generation.xlsx`, and `prompt.xlsx` with new data.
- Adjusted execution counts in `00_master_analysis.ipynb` to correct discrepancies and improve clarity in code execution flow.
- Enhanced error handling for undefined variables in the analysis notebook to prevent runtime issues.
</commit_message>
<xml_diff>
--- a/data/highest_toxicity_records.xlsx
+++ b/data/highest_toxicity_records.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB3"/>
+  <dimension ref="A1:BA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,11 +700,6 @@
           <t>moderation_result</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>max_moderation_score</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -907,9 +902,6 @@
         <v>73</v>
       </c>
       <c r="BA2" t="inlineStr"/>
-      <c r="BB2" t="n">
-        <v>0.3051</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1113,9 +1105,6 @@
         <v>6</v>
       </c>
       <c r="BA3" t="inlineStr"/>
-      <c r="BB3" t="n">
-        <v>0.5073</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1128,7 +1117,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB3"/>
+  <dimension ref="A1:BA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1402,11 +1391,6 @@
           <t>moderation_result</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>max_moderation_score</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1611,9 +1595,6 @@
         <v>0</v>
       </c>
       <c r="BA2" t="inlineStr"/>
-      <c r="BB2" t="n">
-        <v>0.2021</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1827,9 +1808,6 @@
         <v>0</v>
       </c>
       <c r="BA3" t="inlineStr"/>
-      <c r="BB3" t="n">
-        <v>0.2845</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>